<commit_message>
New module "HVAC simulator" added
</commit_message>
<xml_diff>
--- a/files/energy/input/load_emulator/appliance_usage_probability.xlsx
+++ b/files/energy/input/load_emulator/appliance_usage_probability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rollo\Tool\CACER simulator - DEVELOPER\CACER_simulator\files\energy\input\load_emulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/rollo_rse-web_it/Documents/Desktop/CACER simulator - public repo/CACER-simulator/files/energy/input/load_emulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A91C99C-D0A4-423C-9252-3E88993FC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{3A91C99C-D0A4-423C-9252-3E88993FC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F38C70AB-AAEB-4A70-935B-502281B4ACBF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="784" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="784" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_usage_probability" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>time</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Sunday</t>
-  </si>
-  <si>
-    <t>mocrowaves</t>
   </si>
   <si>
     <t>washing_machines</t>
@@ -3812,6 +3809,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3819,7 +3817,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7249,6 +7246,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7256,7 +7254,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8492,15 +8489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>284666</xdr:colOff>
+      <xdr:colOff>288476</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8530,8 +8527,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6477000" y="190500"/>
-          <a:ext cx="12491906" cy="2788920"/>
+          <a:off x="6305550" y="190500"/>
+          <a:ext cx="12499526" cy="2762250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8864,8 +8861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E670C356-3FDE-4B9E-80F9-9F81E3E95366}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98:H98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14209,8 +14206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F7B20C-AA8E-43F7-9935-22301DDB6B97}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14362,7 +14359,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14442,7 +14439,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14459,7 +14456,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -14753,8 +14750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F46834-FBCC-4298-9C5A-BD198B4CEF77}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14770,7 +14767,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
@@ -14798,7 +14795,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>100</v>
@@ -14840,7 +14837,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
         <v>44.3</v>
@@ -14887,19 +14884,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -14907,16 +14904,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -14924,16 +14921,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -14941,16 +14938,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -14958,16 +14955,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -14975,16 +14972,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -14992,16 +14989,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -15009,16 +15006,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -15026,16 +15023,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -15043,16 +15040,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -15060,16 +15057,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -15098,25 +15095,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -15136,10 +15133,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -15159,10 +15156,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -15182,10 +15179,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -15205,10 +15202,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -15228,10 +15225,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -15251,10 +15248,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -15274,10 +15271,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -15297,10 +15294,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -15320,10 +15317,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -15343,10 +15340,10 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>